<commit_message>
DDMIS First Part Complete
DDMIS First Part Complete
</commit_message>
<xml_diff>
--- a/Xen Jakaria/Database Creation For DC8/weblinks.xlsx
+++ b/Xen Jakaria/Database Creation For DC8/weblinks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Designs_All\Xen Jakaria\Database Creation For DC8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7669E4-7B3D-4BC2-A511-27CDDCC1C11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B4FBA8-05C8-4B08-90B0-D05A29728D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Links</t>
   </si>
@@ -55,6 +55,69 @@
   </si>
   <si>
     <t>Dango File uploads and downloads in simple is better than complex</t>
+  </si>
+  <si>
+    <t>https://www.advantch.com/blog/build-a-modern-web-app-using-django-and-javascript/#project-requirements</t>
+  </si>
+  <si>
+    <t>Example of Django Web App Building with Alpine</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/django/index.php</t>
+  </si>
+  <si>
+    <t>w3 Schools Django Web Application Building Step by Step</t>
+  </si>
+  <si>
+    <t>https://learndjango.com/tutorials/template-structure</t>
+  </si>
+  <si>
+    <t>Hosting Application Level Templates in Django</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/django/django_add_static_files.php</t>
+  </si>
+  <si>
+    <t>Hosting Static Files in Django</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GfyP_MYtLng</t>
+  </si>
+  <si>
+    <t>Django Static Files youtube</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=spmFjhQIKOo</t>
+  </si>
+  <si>
+    <t>Debugging Django Project</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/how-to-upload-files-asynchronously-using-jquery/</t>
+  </si>
+  <si>
+    <t>Jquery File Upload</t>
+  </si>
+  <si>
+    <t>Processing File Upload using Jquery Ajax</t>
+  </si>
+  <si>
+    <t>https://itecnote.com/tecnote/ajax-django-ajax-csrf-token-missing/</t>
+  </si>
+  <si>
+    <t>Missing CSRF Token in ajax</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zcJegVlKqqs</t>
+  </si>
+  <si>
+    <t>Django Primary Key in url</t>
+  </si>
+  <si>
+    <t>https://vegibit.com/how-to-use-url-parameters-in-django-routing/</t>
+  </si>
+  <si>
+    <t>How to use URL Parameter in django</t>
   </si>
 </sst>
 </file>
@@ -86,12 +149,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -101,8 +179,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -386,56 +466,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89.5546875" customWidth="1"/>
-    <col min="2" max="2" width="61.88671875" customWidth="1"/>
+    <col min="1" max="1" width="94" customWidth="1"/>
+    <col min="2" max="2" width="60.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -444,6 +612,16 @@
     <hyperlink ref="A3" r:id="rId2" xr:uid="{717AC2C4-823A-4F53-9B9F-15699E4B4147}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{2363D3BD-96DA-4A9E-ACCA-4042ECCA2713}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{4D939174-0EDF-4FBC-9007-8C4A77941020}"/>
+    <hyperlink ref="A6" r:id="rId5" location="project-requirements" xr:uid="{71A7BC44-7A02-4521-9202-C4E3CA904AC6}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{237F48BD-DEF7-457A-9A64-888BBFB2CCB3}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{FF58611D-A6A6-4871-9223-23BECD52775B}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{B131A1F4-7AF1-4E2E-903B-40FA3D6923A8}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{75A67140-FB46-4858-8666-E934130C9799}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{8FA156F7-4B05-4C54-8225-57AE2ED5A6DF}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{04103B3A-DF51-4355-901A-42E047C5E795}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{12F05162-8DD3-4588-942F-7C0F1CBB288F}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{E7511D87-767A-4B56-9D8E-28A64FFAB682}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{2E73FD4A-0B43-47AD-B985-07A441DC73D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User Authentication in website is completed
User Authentication in website is completed
</commit_message>
<xml_diff>
--- a/Xen Jakaria/Database Creation For DC8/weblinks.xlsx
+++ b/Xen Jakaria/Database Creation For DC8/weblinks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Designs_All\Xen Jakaria\Database Creation For DC8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B4FBA8-05C8-4B08-90B0-D05A29728D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D108977B-B156-456E-8457-3B6AD7C040DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Links</t>
   </si>
@@ -118,6 +118,42 @@
   </si>
   <si>
     <t>How to use URL Parameter in django</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sGbzjzO1LHI</t>
+  </si>
+  <si>
+    <t>Django Logging Tutorial youtube</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PL1pc4P-E8TnRehFJPmhQOQCwTdygsxZIx</t>
+  </si>
+  <si>
+    <t>Django Debugging</t>
+  </si>
+  <si>
+    <t>https://betterstack.com/community/guides/logging/how-to-start-logging-with-django/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to Get Started with Logging in Django </t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/logging-in-python-debug-your-django-projects/</t>
+  </si>
+  <si>
+    <t>Logging Getting Started</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Sa_kQheCnds</t>
+  </si>
+  <si>
+    <t>Django Deployment in Linux Server</t>
+  </si>
+  <si>
+    <t>Django Login, Logout, Signup, Password Change, and Password Reset</t>
+  </si>
+  <si>
+    <t>https://learndjango.com/tutorials/django-login-and-logout-tutorial</t>
   </si>
 </sst>
 </file>
@@ -149,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,12 +208,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,6 +232,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -466,15 +520,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="94" customWidth="1"/>
+    <col min="1" max="1" width="105.88671875" customWidth="1"/>
     <col min="2" max="2" width="60.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -604,6 +658,54 @@
       </c>
       <c r="B16" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -622,6 +724,12 @@
     <hyperlink ref="A14" r:id="rId12" xr:uid="{12F05162-8DD3-4588-942F-7C0F1CBB288F}"/>
     <hyperlink ref="A15" r:id="rId13" xr:uid="{E7511D87-767A-4B56-9D8E-28A64FFAB682}"/>
     <hyperlink ref="A16" r:id="rId14" xr:uid="{2E73FD4A-0B43-47AD-B985-07A441DC73D3}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{841E6338-2DEE-4C1D-A271-7C77B768381F}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{9FF21C5B-5AFF-4D1E-A662-F7B5E4EDFF0E}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{33D68685-2A10-42B2-9D74-A3275053C0F7}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{D55B3A34-8F96-4320-A78E-B1B9F079847F}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{843B976F-3F2E-4394-86DA-D3667118D382}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{E8389DFE-1BA0-469B-A3D8-AD3F1F47F7AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>